<commit_message>
fix: programm.cs, add Excel2007 files
</commit_message>
<xml_diff>
--- a/ChromaWrite/ChromaWrite/bin/Debug/Список целевых компонентов Р8.xlsx
+++ b/ChromaWrite/ChromaWrite/bin/Debug/Список целевых компонентов Р8.xlsx
@@ -19,16 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>метан</t>
-  </si>
-  <si>
-    <t>этан</t>
-  </si>
-  <si>
-    <t>пропан</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>i-бутан</t>
   </si>
@@ -70,6 +61,21 @@
   </si>
   <si>
     <t>n-гексан</t>
+  </si>
+  <si>
+    <t>метилциклопентан</t>
+  </si>
+  <si>
+    <t>циклогексан</t>
+  </si>
+  <si>
+    <t>Пропан</t>
+  </si>
+  <si>
+    <t>Метан</t>
+  </si>
+  <si>
+    <t>Этан</t>
   </si>
 </sst>
 </file>
@@ -387,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A17"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,7 +406,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -408,7 +414,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -416,7 +422,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -424,7 +430,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -432,7 +438,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -440,7 +446,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -448,7 +454,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -456,7 +462,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -464,7 +470,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -472,7 +478,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -480,7 +486,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -488,7 +494,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -496,7 +502,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -504,7 +510,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -512,7 +518,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -520,7 +526,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -528,7 +534,23 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>